<commit_message>
Fixing extension URL and name
</commit_message>
<xml_diff>
--- a/source/pages/LAB_LB_FHIR_mapping_and_gaps_for_IG.xlsx
+++ b/source/pages/LAB_LB_FHIR_mapping_and_gaps_for_IG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11715" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UseCase" sheetId="3" r:id="rId1"/>
@@ -1090,17 +1090,6 @@
     <t>Specimen/collection/collected/collectedPeriod/start/@value</t>
   </si>
   <si>
-    <t xml:space="preserve">Extensions:  
-http://build.fhir.org/extension-event-researchstudy.html
-http://build.fhir.org/extension-event-location.html
-</t>
-  </si>
-  <si>
-    <t>Observation extensions: 
-http://build.fhir.org/extension-event-researchstudy.html
-http://build.fhir.org/extension-event-locationhtml</t>
-  </si>
-  <si>
     <t>New extension from Observation:  http://hl7.org/fhir/StructureDefinition/event-note</t>
   </si>
   <si>
@@ -2006,15 +1995,6 @@
 Use the new extension to connect Observation to ResearchStudy.</t>
   </si>
   <si>
-    <t>extension-event-researchstudy  (ref: ResearchStudy.identifier)</t>
-  </si>
-  <si>
-    <t>extension-event-researchstudy  (ref: ResearchStudy.title)</t>
-  </si>
-  <si>
-    <t>extension-event-researchStudy (ref: ResearchStudy.identifier), then ResearchStudy.site (Ref: Location.identifier to Location.managingOrganization Ref: Organization.identifier)</t>
-  </si>
-  <si>
     <t>Extend the FHIR vocabulary to include CDISC values.</t>
   </si>
   <si>
@@ -2111,13 +2091,33 @@
     <t>Provide only one type of result or provide a way to differentiate which results are reported, conventional, or international units.  In some cases, the result unit of measure may provide some indication of whether the results are in conventional or SI.</t>
   </si>
   <si>
-    <t>extension-event-researchstudy  (ref: ResearchStudy..site (ref: Location.identifier to Location.managingOrganization (Ref: Organization.identifier)))</t>
-  </si>
-  <si>
     <t>LBRESU</t>
   </si>
   <si>
     <t>Use a controlled vocabulary list for the toxicity grade. There is not a CDISC standard for this.</t>
+  </si>
+  <si>
+    <t>Observation extensions: 
+http://build.fhir.org/extension-workflow-researchstudy.html
+http://build.fhir.org/extension-event-locationhtml</t>
+  </si>
+  <si>
+    <t>extension-workflow-researchstudy (ref: ResearchStudy.identifier), then ResearchStudy.site (Ref: Location.identifier to Location.managingOrganization Ref: Organization.identifier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extensions:  
+http://build.fhir.org/extension-workflow-researchstudy.html
+http://build.fhir.org/extension-event-location.html
+</t>
+  </si>
+  <si>
+    <t>extension-workflow-researchstudy  (ref: ResearchStudy.identifier)</t>
+  </si>
+  <si>
+    <t>extension-workflow-researchstudy  (ref: ResearchStudy..site (ref: Location.identifier to Location.managingOrganization (Ref: Organization.identifier)))</t>
+  </si>
+  <si>
+    <t>extension-workflow-researchstudy  (ref: ResearchStudy.title)</t>
   </si>
 </sst>
 </file>
@@ -2707,9 +2707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,34 +2728,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>46</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2769,13 +2769,13 @@
         <v>67</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>599</v>
+        <v>634</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>332</v>
+        <v>631</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>68</v>
@@ -2787,7 +2787,7 @@
         <v>51</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2801,13 +2801,13 @@
         <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>600</v>
+        <v>636</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>332</v>
+        <v>631</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>71</v>
@@ -2819,7 +2819,7 @@
         <v>57</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -2836,7 +2836,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>316</v>
@@ -2851,7 +2851,7 @@
         <v>51</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
         <v>33</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>42</v>
@@ -2883,7 +2883,7 @@
         <v>57</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2897,16 +2897,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>332</v>
+        <v>631</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>76</v>
@@ -2915,7 +2915,7 @@
         <v>77</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -2932,7 +2932,7 @@
         <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>42</v>
@@ -2947,7 +2947,7 @@
         <v>57</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2961,13 +2961,13 @@
         <v>82</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>83</v>
@@ -2979,7 +2979,7 @@
         <v>57</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2993,13 +2993,13 @@
         <v>82</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>86</v>
@@ -3011,7 +3011,7 @@
         <v>57</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
@@ -3043,7 +3043,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3054,7 +3054,7 @@
         <v>89</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>92</v>
@@ -3066,7 +3066,7 @@
         <v>301</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>90</v>
@@ -3075,7 +3075,7 @@
         <v>91</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3086,7 +3086,7 @@
         <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>92</v>
@@ -3098,7 +3098,7 @@
         <v>317</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>94</v>
@@ -3107,7 +3107,7 @@
         <v>91</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>92</v>
@@ -3130,7 +3130,7 @@
         <v>317</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>96</v>
@@ -3139,7 +3139,7 @@
         <v>57</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="300" x14ac:dyDescent="0.25">
@@ -3159,10 +3159,10 @@
         <v>42</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>97</v>
@@ -3171,7 +3171,7 @@
         <v>98</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -3188,7 +3188,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>42</v>
@@ -3203,7 +3203,7 @@
         <v>57</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3217,7 +3217,7 @@
         <v>43</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="2" t="s">
@@ -3233,7 +3233,7 @@
         <v>102</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>33</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>42</v>
@@ -3265,7 +3265,7 @@
         <v>57</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>42</v>
@@ -3297,7 +3297,7 @@
         <v>57</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3329,7 +3329,7 @@
         <v>57</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3361,7 +3361,7 @@
         <v>112</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -3375,10 +3375,10 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>510</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>328</v>
@@ -3393,7 +3393,7 @@
         <v>57</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="330" x14ac:dyDescent="0.25">
@@ -3407,10 +3407,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>328</v>
@@ -3425,7 +3425,7 @@
         <v>112</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="360" x14ac:dyDescent="0.25">
@@ -3439,10 +3439,10 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>328</v>
@@ -3457,7 +3457,7 @@
         <v>57</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>33</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>42</v>
@@ -3489,7 +3489,7 @@
         <v>57</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3521,7 +3521,7 @@
         <v>57</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="30" customFormat="1" ht="225" x14ac:dyDescent="0.25">
@@ -3538,7 +3538,7 @@
         <v>33</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>42</v>
@@ -3553,7 +3553,7 @@
         <v>57</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -3570,7 +3570,7 @@
         <v>33</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>42</v>
@@ -3585,7 +3585,7 @@
         <v>57</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3608,7 +3608,7 @@
         <v>131</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>129</v>
@@ -3617,7 +3617,7 @@
         <v>51</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3649,7 +3649,7 @@
         <v>57</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>57</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3713,7 +3713,7 @@
         <v>51</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3727,13 +3727,13 @@
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G32" s="22" t="s">
         <v>42</v>
@@ -3745,7 +3745,7 @@
         <v>57</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -3759,13 +3759,13 @@
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G33" s="22" t="s">
         <v>42</v>
@@ -3777,7 +3777,7 @@
         <v>57</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
         <v>57</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>57</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3855,16 +3855,16 @@
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>152</v>
@@ -3873,7 +3873,7 @@
         <v>57</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3881,7 +3881,7 @@
         <v>136</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>0</v>
@@ -3905,7 +3905,7 @@
         <v>57</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3913,7 +3913,7 @@
         <v>136</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>0</v>
@@ -3937,7 +3937,7 @@
         <v>156</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3945,22 +3945,22 @@
         <v>136</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>154</v>
@@ -3969,7 +3969,7 @@
         <v>57</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3977,13 +3977,13 @@
         <v>136</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>42</v>
@@ -4001,7 +4001,7 @@
         <v>156</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4033,7 +4033,7 @@
         <v>160</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4065,7 +4065,7 @@
         <v>57</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4097,7 +4097,7 @@
         <v>57</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -4111,10 +4111,10 @@
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>58</v>
@@ -4129,7 +4129,7 @@
         <v>57</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4143,10 +4143,10 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>58</v>
@@ -4161,7 +4161,7 @@
         <v>173</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -4175,16 +4175,16 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>174</v>
@@ -4193,7 +4193,7 @@
         <v>57</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4225,7 +4225,7 @@
         <v>178</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4239,7 +4239,7 @@
         <v>179</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>42</v>
@@ -4257,7 +4257,7 @@
         <v>57</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -4274,7 +4274,7 @@
         <v>33</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>42</v>
@@ -4289,7 +4289,7 @@
         <v>57</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="375" x14ac:dyDescent="0.25">
@@ -4303,16 +4303,16 @@
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>184</v>
@@ -4321,7 +4321,7 @@
         <v>51</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
         <v>57</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -4370,7 +4370,7 @@
         <v>33</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>42</v>
@@ -4385,7 +4385,7 @@
         <v>57</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4417,7 +4417,7 @@
         <v>51</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4449,7 +4449,7 @@
         <v>57</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -4481,7 +4481,7 @@
         <v>51</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4513,7 +4513,7 @@
         <v>57</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -4545,7 +4545,7 @@
         <v>57</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -4577,7 +4577,7 @@
         <v>208</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4591,7 +4591,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>42</v>
@@ -4609,7 +4609,7 @@
         <v>57</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4641,7 +4641,7 @@
         <v>216</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>57</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -4687,16 +4687,16 @@
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>224</v>
@@ -4705,7 +4705,7 @@
         <v>57</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -4737,7 +4737,7 @@
         <v>57</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -4751,7 +4751,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>42</v>
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>42</v>
@@ -4815,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>42</v>
@@ -4847,16 +4847,16 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>233</v>
@@ -4865,7 +4865,7 @@
         <v>57</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -4897,7 +4897,7 @@
         <v>57</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="270" x14ac:dyDescent="0.25">
@@ -4914,7 +4914,7 @@
         <v>33</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>42</v>
@@ -4929,7 +4929,7 @@
         <v>57</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -4943,7 +4943,7 @@
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>42</v>
@@ -4961,7 +4961,7 @@
         <v>239</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -4975,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>42</v>
@@ -4993,7 +4993,7 @@
         <v>57</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5025,7 +5025,7 @@
         <v>242</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5033,7 +5033,7 @@
         <v>225</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>0</v>
@@ -5057,7 +5057,7 @@
         <v>246</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5065,7 +5065,7 @@
         <v>225</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>0</v>
@@ -5080,7 +5080,7 @@
         <v>314</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>248</v>
@@ -5089,7 +5089,7 @@
         <v>57</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
         <v>252</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5153,7 +5153,7 @@
         <v>252</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5185,7 +5185,7 @@
         <v>252</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5202,7 +5202,7 @@
         <v>33</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>258</v>
@@ -5234,7 +5234,7 @@
         <v>33</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>258</v>
@@ -5266,7 +5266,7 @@
         <v>33</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>258</v>
@@ -5304,7 +5304,7 @@
         <v>262</v>
       </c>
       <c r="G81" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>260</v>
@@ -5313,7 +5313,7 @@
         <v>57</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -5336,7 +5336,7 @@
         <v>262</v>
       </c>
       <c r="G82" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>260</v>
@@ -5345,7 +5345,7 @@
         <v>57</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -5368,7 +5368,7 @@
         <v>262</v>
       </c>
       <c r="G83" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>260</v>
@@ -5377,7 +5377,7 @@
         <v>57</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -5400,7 +5400,7 @@
         <v>269</v>
       </c>
       <c r="G84" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>267</v>
@@ -5409,7 +5409,7 @@
         <v>57</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -5432,7 +5432,7 @@
         <v>269</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>267</v>
@@ -5441,7 +5441,7 @@
         <v>57</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -5464,7 +5464,7 @@
         <v>269</v>
       </c>
       <c r="G86" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>267</v>
@@ -5473,7 +5473,7 @@
         <v>57</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5487,7 +5487,7 @@
         <v>0</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>42</v>
@@ -5505,7 +5505,7 @@
         <v>275</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5519,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>42</v>
@@ -5537,7 +5537,7 @@
         <v>275</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5551,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>42</v>
@@ -5569,7 +5569,7 @@
         <v>275</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5601,7 +5601,7 @@
         <v>57</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5633,7 +5633,7 @@
         <v>57</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5665,7 +5665,7 @@
         <v>57</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -5682,7 +5682,7 @@
         <v>42</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>324</v>
@@ -5697,7 +5697,7 @@
         <v>51</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -5705,7 +5705,7 @@
         <v>225</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>0</v>
@@ -5714,7 +5714,7 @@
         <v>33</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>42</v>
@@ -5723,13 +5723,13 @@
         <v>42</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I94" s="33" t="s">
         <v>51</v>
       </c>
       <c r="J94" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5746,7 +5746,7 @@
         <v>33</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>52</v>
@@ -5761,7 +5761,7 @@
         <v>51</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5778,7 +5778,7 @@
         <v>33</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>55</v>
@@ -5793,7 +5793,7 @@
         <v>51</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5810,7 +5810,7 @@
         <v>33</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>58</v>
@@ -5825,7 +5825,7 @@
         <v>57</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5842,7 +5842,7 @@
         <v>33</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>61</v>
@@ -5857,7 +5857,7 @@
         <v>51</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5874,7 +5874,7 @@
         <v>33</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>61</v>
@@ -5889,7 +5889,7 @@
         <v>57</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -5902,9 +5902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5920,16 +5920,16 @@
   <sheetData>
     <row r="1" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E1" s="27" t="s">
         <v>46</v>
@@ -5941,13 +5941,13 @@
         <v>44</v>
       </c>
       <c r="H1" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>358</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>359</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5958,13 +5958,13 @@
         <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>599</v>
+        <v>634</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>332</v>
+        <v>631</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>68</v>
@@ -5973,13 +5973,13 @@
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -5990,28 +5990,28 @@
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>601</v>
+        <v>632</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>331</v>
+        <v>633</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -6022,13 +6022,13 @@
         <v>82</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>83</v>
@@ -6037,18 +6037,18 @@
         <v>25</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>26</v>
@@ -6067,13 +6067,13 @@
         <v>23</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -6094,16 +6094,16 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -6114,10 +6114,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>510</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>328</v>
@@ -6127,13 +6127,13 @@
         <v>113</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>113</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -6157,18 +6157,18 @@
         <v>123</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>123</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>0</v>
@@ -6190,15 +6190,15 @@
         <v>42</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>0</v>
@@ -6220,21 +6220,21 @@
         <v>42</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>42</v>
@@ -6242,27 +6242,27 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="8" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>42</v>
@@ -6272,27 +6272,27 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>42</v>
@@ -6302,16 +6302,16 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -6322,31 +6322,31 @@
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>318</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>153</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>0</v>
@@ -6355,23 +6355,23 @@
         <v>165</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>166</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -6382,40 +6382,40 @@
         <v>0</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -6423,7 +6423,7 @@
         <v>288</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>42</v>
@@ -6434,13 +6434,13 @@
     </row>
     <row r="18" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>42</v>
@@ -6448,21 +6448,21 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="17" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>293</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>0</v>
@@ -6476,46 +6476,46 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="8" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>295</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>179</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>182</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -6523,46 +6523,46 @@
         <v>5</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6" t="s">
@@ -6572,21 +6572,21 @@
         <v>42</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>406</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>408</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>42</v>
@@ -6602,15 +6602,15 @@
         <v>42</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>0</v>
@@ -6635,12 +6635,12 @@
         <v>200</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>0</v>
@@ -6659,13 +6659,13 @@
         <v>217</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>217</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -6689,24 +6689,24 @@
         <v>193</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>193</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>42</v>
@@ -6716,16 +6716,16 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>291</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -6736,7 +6736,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>42</v>
@@ -6752,19 +6752,19 @@
         <v>42</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>42</v>
@@ -6772,27 +6772,27 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>42</v>
@@ -6802,16 +6802,16 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -6828,20 +6828,20 @@
         <v>42</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="8" t="s">
         <v>264</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>264</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -6858,55 +6858,55 @@
         <v>42</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="8" t="s">
         <v>271</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>271</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="8" t="s">
         <v>289</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I33" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="J33" s="8" t="s">
         <v>432</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>0</v>
@@ -6922,21 +6922,21 @@
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>0</v>
@@ -6952,16 +6952,16 @@
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -6972,7 +6972,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>42</v>
@@ -6982,81 +6982,81 @@
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>278</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="8" t="s">
         <v>287</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="H38" s="8" t="s">
         <v>439</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>441</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>290</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>0</v>
@@ -7068,23 +7068,23 @@
         <v>42</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="29" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
@@ -7098,7 +7098,7 @@
     </row>
     <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>42</v>
@@ -7119,18 +7119,18 @@
         <v>298</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>298</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>26</v>
@@ -7157,12 +7157,12 @@
         <v>27</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>0</v>
@@ -7171,7 +7171,7 @@
         <v>33</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>42</v>
@@ -7183,18 +7183,18 @@
         <v>294</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>294</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>0</v>
@@ -7206,33 +7206,33 @@
         <v>42</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>285</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>285</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>42</v>
@@ -7247,27 +7247,27 @@
         <v>297</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>297</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>42</v>
@@ -7282,10 +7282,10 @@
         <v>42</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -7299,7 +7299,7 @@
         <v>33</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>42</v>
@@ -7317,12 +7317,12 @@
         <v>284</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>0</v>
@@ -7331,7 +7331,7 @@
         <v>33</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="E48" s="24" t="s">
         <v>42</v>
@@ -7346,15 +7346,15 @@
         <v>42</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>0</v>
@@ -7363,7 +7363,7 @@
         <v>33</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>42</v>
@@ -7378,10 +7378,10 @@
         <v>42</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>